<commit_message>
implement batch import of controls
</commit_message>
<xml_diff>
--- a/storage/app/import-templates/reagents.xlsx
+++ b/storage/app/import-templates/reagents.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sparclex/code/nova/storage/app/import-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sparclex/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A69196-1247-484A-B1C6-C0C949A20282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860C0F50-09D4-BA43-9FFD-3DD6F374B2DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="960" windowWidth="27840" windowHeight="16600" xr2:uid="{BC5B3249-C409-9B41-A5F0-8EA98CCB03B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>lot</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>supplier</t>
   </si>
 </sst>
 </file>
@@ -389,15 +395,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BC6ADB-F496-F143-845F-4FAFEC5448F7}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +416,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>

</xml_diff>